<commit_message>
queries - ranking - rec
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
@@ -1066,7 +1066,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>711694.622</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>711694.622</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>711694.622</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>711694.622</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>711694.622</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>711694.622</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>168839.343</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>168839.343</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>66.2</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>66.2</v>

</xml_diff>

<commit_message>
início das queries de análise serial
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
@@ -1066,7 +1066,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>711694.622</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>711694.622</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>711694.622</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>711694.622</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>711694.622</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>66.2</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>66.2</v>

</xml_diff>

<commit_message>
geração de análises seriais
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
@@ -1122,7 +1122,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>415470.057</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>415470.057</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>66.2</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>66.2</v>

</xml_diff>

<commit_message>
fixar o banco de dados de autoria e mencoes no ano de análise
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
@@ -1066,7 +1066,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>711694.622</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>711694.622</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>711694.622</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>711694.622</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>711694.622</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>711694.622</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>168839.343</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>168839.343</v>

</xml_diff>

<commit_message>
gerar conteúdo por módulo de análise
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-categoria-mencao-tdn.xlsx
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>711694.622</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>711694.622</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>415470.057</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>415470.057</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>168839.343</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>168839.343</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>66.2</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>66.2</v>

</xml_diff>